<commit_message>
update files for sprint2
</commit_message>
<xml_diff>
--- a/documents/Acceptance Criteria.xlsx
+++ b/documents/Acceptance Criteria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raffertyleung/Desktop/cs691/2023S-Leung/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C897DF9B-BF29-354B-90A4-DF3D6D456404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69771840-B0EE-9E4E-80E9-A2D229B39E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" xr2:uid="{F9CDC593-2F19-A54B-AEAD-F02075CEF372}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$22</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>User Story ID</t>
   </si>
@@ -171,6 +171,12 @@
   </si>
   <si>
     <t>Then I want this page tell me what my results mean</t>
+  </si>
+  <si>
+    <t>Scenario: User sends photo</t>
+  </si>
+  <si>
+    <t>Scenario: User has questions</t>
   </si>
 </sst>
 </file>
@@ -544,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E49277-683F-2045-B002-83C29298E6B5}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -729,7 +735,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -743,27 +749,31 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
       <c r="B24" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
       <c r="B25" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
       <c r="B26" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
       <c r="B27" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B28" t="s">
@@ -777,27 +787,31 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
       <c r="B29" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
       <c r="B30" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
       <c r="B31" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
       <c r="B32" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B33" s="4" t="s">
@@ -811,48 +825,69 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
       <c r="B34" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B35" s="4" t="s">
+    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="B36" s="4" t="s">
+    <row r="37" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="38" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>35</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B38" s="4" t="s">
+    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B39" s="4" t="s">
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+      <c r="B41" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="B40" s="4" t="s">
+    <row r="42" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+      <c r="B42" s="4" t="s">
         <v>42</v>
       </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>